<commit_message>
simplified excel to json process. add skills display and data import.
</commit_message>
<xml_diff>
--- a/heroes.xlsx
+++ b/heroes.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nantas/projects/tbc/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="560" windowWidth="25040" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="2340" yWindow="1900" windowWidth="25040" windowHeight="16980" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="heroes" sheetId="1" r:id="rId1"/>
+    <sheet name="activeskills" sheetId="2" r:id="rId2"/>
+    <sheet name="passiveskills" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -229,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="120">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -388,6 +395,725 @@
   </si>
   <si>
     <t>0.5|0.05</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>base1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>base2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseInc_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseInc_2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HealOne</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HealAll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blizzard</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeathTouch</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beam</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slashes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeathTouch</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>StunHammer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>治疗之光</t>
+    <rPh sb="0" eb="1">
+      <t>zhi'l</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>zhi'guang</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>治疗之风</t>
+    <rPh sb="0" eb="1">
+      <t>zhi'liao</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>zhi'feng</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴风雪</t>
+    <rPh sb="0" eb="1">
+      <t>bao'feng'xue</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡一击</t>
+    <rPh sb="0" eb="1">
+      <t>si'w</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yi'ji</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>赤红射线</t>
+    <rPh sb="0" eb="1">
+      <t>chi'hong</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>she'xian</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>终极武器</t>
+    <rPh sb="0" eb="1">
+      <t>zhong'ji</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>wu'qi</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>黎明之锤</t>
+    <rPh sb="0" eb="1">
+      <t>li'ming'zhi'chui</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtkUpSelf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtkUpAll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ApUpSelf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ApUpAll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveUpAll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LeechAll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HasteAll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegenAll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>base1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseInc_2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击上升</t>
+    <rPh sb="0" eb="1">
+      <t>gong'ji</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>shang'sh</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击光环</t>
+    <rPh sb="0" eb="1">
+      <t>gong'ji</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>guang'huan</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>法力之源</t>
+    <rPh sb="0" eb="1">
+      <t>fa'li</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>zhi'yuan</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>法力光环</t>
+    <rPh sb="0" eb="1">
+      <t>fa'li</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>guang'h</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>移速光环</t>
+    <rPh sb="0" eb="1">
+      <t>yi'su</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>guang'h</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸血光环</t>
+    <rPh sb="0" eb="1">
+      <t>xi'xue</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>guang'huan</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻速光环</t>
+    <rPh sb="0" eb="1">
+      <t>gong'su</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>guang'h</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复光环</t>
+    <rPh sb="0" eb="1">
+      <t>hui'fu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>guang'h</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>自身攻击力提高 ${1}%</t>
+    <rPh sb="0" eb="1">
+      <t>zi'shen</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>gong'ji</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>li'ti'gao</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>自身法力强度提高 ${1}%</t>
+    <rPh sb="0" eb="1">
+      <t>zi'shen</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>fa'li</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>qiang'du</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ti'gao</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>队伍全体攻击力提高 ${1}%</t>
+    <rPh sb="0" eb="1">
+      <t>dui'wu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>quan'ti</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>gong'ji'li</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ti'gao</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>队伍全体法力强度提高 ${1}%</t>
+    <rPh sb="0" eb="1">
+      <t>dui'wu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>quan'ti</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>fa'li</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>qiang'du</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ti'gao</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>队伍全体移动速度提高 ${1}%</t>
+    <rPh sb="0" eb="1">
+      <t>dui'wu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>quan'ti</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>yi'dong</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>su'du</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ti'gao</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>队伍全体攻击回复造成伤害的 ${1}%</t>
+    <rPh sb="0" eb="1">
+      <t>dui'wu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>quan'ti</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>gong'ji</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>hui'fu</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>zao'ch</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>shang'hai</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>de</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>队伍全体攻击和技能施放速度提高 ${1}%</t>
+    <rPh sb="0" eb="1">
+      <t>dui'wu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>quan'ti</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>gong'ji'su'du</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>he</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ji'neng</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>shi'fang</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>su'du</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ti'gao</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>队伍全体每秒恢复 ${1} 点生命</t>
+    <rPh sb="0" eb="1">
+      <t>dui'wu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>quan'ti</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>mei</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>miao'hui'fu</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>dian</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>sheng'm</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复当前英雄生命值 ${1} 点</t>
+    <rPh sb="0" eb="1">
+      <t>hui'fu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>dang'q</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ying'x</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>sheng'm'z</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>dian</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复队伍全体生命值 ${1} 点</t>
+    <rPh sb="0" eb="1">
+      <t>hui'fu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>dui'wu</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>quan'ti</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>sheng'm'z</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>dian</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>向前冲刺，对第一个遇到的敌人造成 ${1} 点伤害</t>
+    <rPh sb="0" eb="1">
+      <t>xiang</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>qian</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>chong'ji</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ci</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>dui</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>di'yi'ge</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>yu'dao</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>d</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>di'r</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>zao'ch</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>dian</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>shang'h</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤3波暴风雪，每波造成 ${1} 点伤害，对命中目标产生 0.5 秒定身效果</t>
+    <rPh sb="0" eb="1">
+      <t>zhao'h</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>bo</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>bao'feng'xue</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>zao'ch</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>dian</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>shang'h</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>dui</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ming'zhong</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>mu'b</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>chan's</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>miao</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ding'shen</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>xiao'g</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>向前方发射射线，总共造成 ${1} 点伤害</t>
+    <rPh sb="0" eb="1">
+      <t>xiang</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>qian</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>fang</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>fa'she</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>she'x</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>zong'g</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>zao'ch</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>dian</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>shang'h</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>向前方发动多次攻击，共造成 ${1} 点伤害</t>
+    <rPh sb="0" eb="1">
+      <t>xiang</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>qian'fang</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>fa'dong</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>duo'ci</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>gong'ji</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>gong</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>zao'ch</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>dian</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>shang'h</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>向前方发动攻击，造成 ${1} 点伤害并眩晕目标 1秒</t>
+    <rPh sb="0" eb="1">
+      <t>xiang'qian'fang</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>fa'dong</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>gong'ji</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>zao'ch</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>dian</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>shang'hai</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>xuan'yun</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>mu'b</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>miao</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>prepare</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_1011</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_3090</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_4000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_1000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_18800</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_1340</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_16300</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_1010</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_1030</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_1110</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_1510</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_17700</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_1100</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_12100</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_icons.plist/skill_16600</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blizzard</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slashes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beam</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtkUpSelf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HasteAll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ApUpSelf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ApUpAll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtkUpAll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -395,7 +1121,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -434,6 +1160,24 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -452,10 +1196,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -463,12 +1209,22 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -796,11 +1552,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="13.1640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="4" customWidth="1"/>
@@ -811,7 +1567,7 @@
     <col min="11" max="11" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -846,7 +1602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -871,11 +1627,15 @@
       <c r="H2" s="1">
         <v>50</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -900,11 +1660,15 @@
       <c r="H3" s="1">
         <v>80</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -929,11 +1693,15 @@
       <c r="H4" s="1">
         <v>70</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -958,11 +1726,15 @@
       <c r="H5" s="1">
         <v>70</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -987,11 +1759,15 @@
       <c r="H6" s="1">
         <v>50</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1016,8 +1792,14 @@
       <c r="H7" s="1">
         <v>120</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="I7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1042,8 +1824,14 @@
       <c r="H8" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="I8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1067,16 +1855,457 @@
       </c>
       <c r="H9" s="1">
         <v>40</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J9" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="44.5" style="5" customWidth="1"/>
+    <col min="9" max="9" width="29.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2">
+        <v>300</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="F3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>0.5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>150</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5">
+        <v>600</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6">
+        <v>400</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+      <c r="H6">
+        <v>0.4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7">
+        <v>500</v>
+      </c>
+      <c r="F7">
+        <v>80</v>
+      </c>
+      <c r="H7">
+        <v>0.2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8">
+        <v>250</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>0.5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="8" max="8" width="33.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+      <c r="F3">
+        <v>0.2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="F5">
+        <v>0.2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to new asset loading api
</commit_message>
<xml_diff>
--- a/heroes.xlsx
+++ b/heroes.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nantas/projects/tbc/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1900" windowWidth="25040" windowHeight="16980" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="heroes" sheetId="1" r:id="rId1"/>
@@ -1021,66 +1016,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>skill_icons.plist/skill_1011</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_3090</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_4000</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_1000</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_18800</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_1340</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_16300</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_1010</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_1030</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_1110</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_1510</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_17700</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_1100</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_12100</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill_icons.plist/skill_16600</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Blizzard</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1115,6 +1050,58 @@
   <si>
     <t>cost</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_1340</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_4000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_18800</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_1000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_1011</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_3090</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_16300</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_1010</t>
+  </si>
+  <si>
+    <t>skill_1030</t>
+  </si>
+  <si>
+    <t>skill_1110</t>
+  </si>
+  <si>
+    <t>skill_1510</t>
+  </si>
+  <si>
+    <t>skill_17700</t>
+  </si>
+  <si>
+    <t>skill_1100</t>
+  </si>
+  <si>
+    <t>skill_12100</t>
+  </si>
+  <si>
+    <t>skill_16600</t>
   </si>
 </sst>
 </file>
@@ -1214,9 +1201,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1556,7 +1543,7 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="4" max="4" width="13.1640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="4" customWidth="1"/>
@@ -1567,7 +1554,7 @@
     <col min="11" max="11" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1602,7 +1589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1631,11 +1618,11 @@
         <v>52</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1668,7 +1655,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1697,11 +1684,11 @@
         <v>53</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1727,14 +1714,14 @@
         <v>70</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>65</v>
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1763,11 +1750,11 @@
         <v>50</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1793,13 +1780,13 @@
         <v>120</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1828,10 +1815,10 @@
         <v>46</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1857,7 +1844,7 @@
         <v>40</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="J9" t="s">
         <v>66</v>
@@ -1867,6 +1854,11 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1874,17 +1866,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="44.5" style="5" customWidth="1"/>
     <col min="9" max="9" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1913,10 +1905,10 @@
         <v>95</v>
       </c>
       <c r="J1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1936,13 +1928,13 @@
         <v>0.5</v>
       </c>
       <c r="I2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="J2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1962,13 +1954,13 @@
         <v>0.5</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="J3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="30">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1988,13 +1980,13 @@
         <v>0.5</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="J4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="30">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2014,13 +2006,13 @@
         <v>0.1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="J5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -2040,13 +2032,13 @@
         <v>0.4</v>
       </c>
       <c r="I6" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="J6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -2066,13 +2058,13 @@
         <v>0.2</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="J7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="30">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -2092,7 +2084,7 @@
         <v>0.5</v>
       </c>
       <c r="I8" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="J8">
         <v>3</v>
@@ -2101,6 +2093,11 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2108,17 +2105,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="8" max="8" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2144,7 +2141,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -2161,10 +2158,10 @@
         <v>0.5</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -2181,10 +2178,10 @@
         <v>0.2</v>
       </c>
       <c r="H3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -2201,10 +2198,10 @@
         <v>0.5</v>
       </c>
       <c r="H4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -2221,10 +2218,10 @@
         <v>0.2</v>
       </c>
       <c r="H5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -2241,10 +2238,10 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -2261,10 +2258,10 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -2281,10 +2278,10 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -2301,11 +2298,16 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update team build demo
</commit_message>
<xml_diff>
--- a/heroes.xlsx
+++ b/heroes.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nantas/projects/demo-team-build-ui/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="6400" yWindow="3760" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="heroes" sheetId="1" r:id="rId1"/>
@@ -80,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -158,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -184,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -231,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="159">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -241,38 +246,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>夏洛特</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>弗格斯</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>李山</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>皮塔娜</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>恩布拉</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>派洛尔</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>希格非</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>素子</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>class</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -301,66 +274,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Tank</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Assasin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Shooter</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Shooter</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wizard</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Support</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Assasin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>-2.5|-76.8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>62|-77</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>22|-131</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>68|-80</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>12|-74</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>-5|-91</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>26|-94</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>-16|-118</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>iconPos</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -369,30 +286,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>0.45|0.1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>0.5|0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>0.4|0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.45|0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.4|0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.5|0.05</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -438,10 +335,6 @@
   </si>
   <si>
     <t>Slashes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeathTouch</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1102,6 +995,274 @@
   </si>
   <si>
     <t>skill_16600</t>
+  </si>
+  <si>
+    <t>3|-97</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sierokarte</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Christina</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deliford</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Teluse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Io</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mary</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magisa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>43|-223</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-61|-113</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wizard</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tank</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-13|-198</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-7|-82</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>16|-185</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wizard</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>42|-201</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assasin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>115|-187</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tank</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-39|-184</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shooter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>74|-179</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>8|-150</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vira</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assasin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gayne</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assasin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ange</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Teena</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shooter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rosamia</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tank</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lily</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wizard</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Volemia</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5|0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>portraitScale</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.4|0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.6|0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.45|0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.35|0.05</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.85</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.6|0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.35|0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.45|0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.95</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.55|0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HealAll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HealOne</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slashes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>StunHammer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>64|-144</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-24|-228</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>24|-196</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5|0.05</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.75</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.55|0.05</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.48|0.02</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1201,9 +1362,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1537,24 +1698,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="13.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" customWidth="1"/>
-    <col min="11" max="11" width="14.5" customWidth="1"/>
+    <col min="4" max="5" width="13.1640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1562,303 +1723,535 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>127</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="1">
-        <v>800</v>
+        <v>130</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="G2" s="1">
-        <v>120</v>
+        <v>1100</v>
       </c>
       <c r="H2" s="1">
+        <v>90</v>
+      </c>
+      <c r="I2" s="1">
         <v>50</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1000</v>
+        <v>132</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="G3" s="1">
-        <v>80</v>
+        <v>800</v>
       </c>
       <c r="H3" s="1">
-        <v>80</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="I3" s="1">
+        <v>150</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="K3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1100</v>
+        <v>133</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="G4" s="1">
-        <v>90</v>
+        <v>750</v>
       </c>
       <c r="H4" s="1">
-        <v>70</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
+      </c>
+      <c r="I4" s="1">
+        <v>130</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11">
+        <v>148</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="1">
-        <v>750</v>
+        <v>130</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="G5" s="1">
+        <v>850</v>
+      </c>
+      <c r="H5" s="1">
         <v>100</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>70</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11">
+        <v>70</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>28</v>
+        <v>151</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="1">
-        <v>700</v>
+        <v>158</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="G6" s="1">
-        <v>90</v>
+        <v>800</v>
       </c>
       <c r="H6" s="1">
-        <v>50</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="I6" s="1">
+        <v>125</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11">
+        <v>68</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="1">
-        <v>750</v>
+        <v>137</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="G7" s="1">
-        <v>50</v>
+        <v>900</v>
       </c>
       <c r="H7" s="1">
         <v>120</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>96</v>
+      <c r="I7" s="1">
+        <v>50</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>149</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="1">
-        <v>850</v>
+        <v>136</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="G8" s="1">
-        <v>50</v>
+        <v>1200</v>
       </c>
       <c r="H8" s="1">
-        <v>100</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>46</v>
+        <v>95</v>
+      </c>
+      <c r="I8" s="1">
+        <v>60</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>19</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G9" s="1">
+        <v>720</v>
+      </c>
+      <c r="H9" s="1">
+        <v>110</v>
+      </c>
+      <c r="I9" s="1">
+        <v>75</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="B10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G10" s="1">
+        <v>880</v>
+      </c>
+      <c r="H10" s="1">
+        <v>135</v>
+      </c>
+      <c r="I10" s="1">
+        <v>90</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" s="1">
         <v>850</v>
       </c>
-      <c r="G9" s="1">
-        <v>110</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="H11" s="1">
+        <v>125</v>
+      </c>
+      <c r="I11" s="1">
+        <v>70</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="J9" t="s">
-        <v>66</v>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G12" s="1">
+        <v>950</v>
+      </c>
+      <c r="H12" s="1">
+        <v>120</v>
+      </c>
+      <c r="I12" s="1">
+        <v>40</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G13" s="1">
+        <v>800</v>
+      </c>
+      <c r="H13" s="1">
+        <v>105</v>
+      </c>
+      <c r="I13" s="1">
+        <v>65</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1050</v>
+      </c>
+      <c r="H14" s="1">
+        <v>95</v>
+      </c>
+      <c r="I14" s="1">
+        <v>90</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G15" s="1">
+        <v>700</v>
+      </c>
+      <c r="H15" s="1">
+        <v>60</v>
+      </c>
+      <c r="I15" s="1">
+        <v>160</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1870,53 +2263,53 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="44.5" style="5" customWidth="1"/>
     <col min="9" max="9" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="J1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="D2">
         <v>300</v>
@@ -1928,21 +2321,21 @@
         <v>0.5</v>
       </c>
       <c r="I2" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="J2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D3">
         <v>200</v>
@@ -1954,21 +2347,21 @@
         <v>0.5</v>
       </c>
       <c r="I3" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="J3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="D4">
         <v>150</v>
@@ -1980,21 +2373,21 @@
         <v>0.5</v>
       </c>
       <c r="I4" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="J4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="D5">
         <v>600</v>
@@ -2006,21 +2399,21 @@
         <v>0.1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="J5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>400</v>
@@ -2032,21 +2425,21 @@
         <v>0.4</v>
       </c>
       <c r="I6" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="J6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="D7">
         <v>500</v>
@@ -2058,21 +2451,21 @@
         <v>0.2</v>
       </c>
       <c r="I7" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="J7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="D8">
         <v>250</v>
@@ -2084,7 +2477,7 @@
         <v>0.5</v>
       </c>
       <c r="I8" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="J8">
         <v>3</v>
@@ -2093,11 +2486,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2105,17 +2493,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="8" max="8" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2123,33 +2511,33 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
-        <v>69</v>
-      </c>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>71</v>
-      </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2158,18 +2546,18 @@
         <v>0.5</v>
       </c>
       <c r="H2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <v>0.5</v>
@@ -2178,18 +2566,18 @@
         <v>0.2</v>
       </c>
       <c r="H3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2198,18 +2586,18 @@
         <v>0.5</v>
       </c>
       <c r="H4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>0.5</v>
@@ -2218,18 +2606,18 @@
         <v>0.2</v>
       </c>
       <c r="H5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2238,18 +2626,18 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -2258,18 +2646,18 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2278,18 +2666,18 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2298,16 +2686,11 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>